<commit_message>
Fill modalities for review
</commit_message>
<xml_diff>
--- a/sample_data/annotation/01/phase2/upload/8141.xlsx
+++ b/sample_data/annotation/01/phase2/upload/8141.xlsx
@@ -258,6 +258,9 @@
     <t xml:space="preserve">Mit Ausnahme der als Gemischtes Baugebiet/Betriebsbaugebiet gewidmeten Flächen sind bebaubare jedoch unbebaut bleibende Grundflächen gärtnerisch auszugestalten.</t>
   </si>
   <si>
+    <t xml:space="preserve">permission</t>
+  </si>
+  <si>
     <t xml:space="preserve">AusnahmeGaertnerischAuszugestaltende</t>
   </si>
   <si>
@@ -312,6 +315,9 @@
     <t xml:space="preserve">Für die mit BB2 bezeichneten Grundflächen wird bestimmt: Die zur Errichtung gelangenden Dächer von Gebäuden mit einer bebauten Fläche von mehr als 12 m² sind als Flachdächer auszuführen und entsprechend dem Stand der Technik zu begrünen.</t>
   </si>
   <si>
+    <t xml:space="preserve">contentException</t>
+  </si>
+  <si>
     <t xml:space="preserve">BB2</t>
   </si>
   <si>
@@ -408,9 +414,6 @@
     <t xml:space="preserve">AnOeffentlichenVerkehrsflaechen</t>
   </si>
   <si>
-    <t xml:space="preserve">permission</t>
-  </si>
-  <si>
     <t xml:space="preserve">BauklasseVIHoeheMin</t>
   </si>
   <si>
@@ -445,9 +448,6 @@
   </si>
   <si>
     <t xml:space="preserve">GelaendeneigungMin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contentException</t>
   </si>
   <si>
     <t xml:space="preserve">FBOKMinimumWohnungen</t>
@@ -965,7 +965,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="64.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1562,13 +1562,13 @@
         <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>53</v>
@@ -1577,7 +1577,7 @@
         <v>54</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>31</v>
@@ -1586,7 +1586,7 @@
         <v>60</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>63</v>
@@ -1600,10 +1600,10 @@
     </row>
     <row r="18" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>27</v>
@@ -1612,7 +1612,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>63</v>
@@ -1621,32 +1621,32 @@
         <v>64</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>60</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
@@ -1666,10 +1666,10 @@
     </row>
     <row r="21" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
@@ -1681,7 +1681,7 @@
         <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>31</v>
@@ -1690,15 +1690,15 @@
         <v>60</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>27</v>
@@ -1713,7 +1713,7 @@
         <v>30</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>41</v>
@@ -1758,7 +1758,7 @@
         <v>37</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="W22" s="3" t="s">
         <v>31</v>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="23" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3241,7 +3241,7 @@
       <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="73.55"/>
@@ -3278,10 +3278,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>53</v>
@@ -3290,25 +3290,25 @@
         <v>44</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>63</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>60</v>
@@ -3336,37 +3336,37 @@
         <v>53</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="8" t="s">
         <v>42</v>
@@ -3381,98 +3381,98 @@
         <v>50</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="11" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="U5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>27</v>
@@ -3533,7 +3533,7 @@
         <v>148</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>149</v>
@@ -3553,7 +3553,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>153</v>
@@ -3571,7 +3571,7 @@
         <v>157</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>158</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>164</v>
@@ -3645,7 +3645,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>173</v>
@@ -3654,12 +3654,12 @@
         <v>174</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>175</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P19" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add numbering for attributes
</commit_message>
<xml_diff>
--- a/sample_data/annotation/01/phase2/upload/8141.xlsx
+++ b/sample_data/annotation/01/phase2/upload/8141.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="186">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t xml:space="preserve">AusnahmeGaertnerischAuszugestaltende</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> unbebaut bleibende Grundflächen</t>
   </si>
   <si>
     <t xml:space="preserve">AnordnungGaertnerischeAusgestaltung</t>
@@ -961,11 +958,11 @@
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="64.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1570,23 +1567,11 @@
       <c r="E17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="L17" s="1" t="s">
         <v>60</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>63</v>
@@ -1600,10 +1585,10 @@
     </row>
     <row r="18" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>27</v>
@@ -1612,7 +1597,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>63</v>
@@ -1621,15 +1606,15 @@
         <v>64</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>72</v>
@@ -1638,15 +1623,15 @@
         <v>60</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
@@ -1666,10 +1651,10 @@
     </row>
     <row r="21" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
@@ -1681,7 +1666,7 @@
         <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>31</v>
@@ -1690,15 +1675,15 @@
         <v>60</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>27</v>
@@ -1713,7 +1698,7 @@
         <v>30</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>41</v>
@@ -1758,7 +1743,7 @@
         <v>37</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W22" s="3" t="s">
         <v>31</v>
@@ -1766,10 +1751,10 @@
     </row>
     <row r="23" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3278,10 +3263,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>53</v>
@@ -3290,25 +3275,25 @@
         <v>44</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="L3" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>63</v>
       </c>
       <c r="N3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>60</v>
@@ -3336,37 +3321,37 @@
         <v>53</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="O4" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="P4" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q4" s="8" t="s">
         <v>42</v>
@@ -3381,48 +3366,48 @@
         <v>50</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="S5" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="U5" s="8" t="s">
         <v>31</v>
@@ -3433,46 +3418,46 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="Q6" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="R6" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="S6" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="S6" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="U6" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>27</v>
@@ -3483,37 +3468,37 @@
         <v>44</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>142</v>
       </c>
       <c r="Q7" s="8" t="s">
         <v>49</v>
       </c>
       <c r="R7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="S7" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="U7" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3524,57 +3509,57 @@
         <v>45</v>
       </c>
       <c r="I8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="L8" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="M8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="M8" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="O8" s="8" t="s">
+      <c r="P8" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>68</v>
       </c>
       <c r="R8" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="S8" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="S8" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="M9" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="O9" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>73</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>37</v>
@@ -3585,48 +3570,48 @@
         <v>63</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>64</v>
       </c>
       <c r="O10" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="P10" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="Q10" s="8" t="s">
         <v>51</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H11" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="O11" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="P11" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="Q11" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="S11" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3634,46 +3619,46 @@
         <v>32</v>
       </c>
       <c r="H12" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="P12" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>174</v>
-      </c>
       <c r="P13" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I14" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>178</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>61</v>
@@ -3682,47 +3667,47 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="11"/>
       <c r="P16" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P17" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P18" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P19" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P20" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P21" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P22" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P23" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P24" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>